<commit_message>
Create API to download the Excel for data loading services and specialities
</commit_message>
<xml_diff>
--- a/backend/resources/examples/CARGA ESPECIALIDADES EXTERNAS.xlsx
+++ b/backend/resources/examples/CARGA ESPECIALIDADES EXTERNAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\PortableApps\Documents\Projects\sinasuite-dl\backend\resources\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47728DD6-6857-4B81-97F3-5EBAFD863F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F63FE6-CA5A-4836-9EDC-CDEC70668708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>CAMPOS DEL EXCEL</t>
   </si>
@@ -83,18 +83,6 @@
   </si>
   <si>
     <t>Si esta vacio, se aplicara para todo los centros externos</t>
-  </si>
-  <si>
-    <t>ORTOPEDIA Y TRAUMATOLOGIA INFANTIL</t>
-  </si>
-  <si>
-    <t>OTI</t>
-  </si>
-  <si>
-    <t>UNIDAD DE TRANSPLANTE PULMONAR</t>
-  </si>
-  <si>
-    <t>UTP</t>
   </si>
 </sst>
 </file>
@@ -457,10 +445,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,34 +480,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>